<commit_message>
[UPD] 更新 Dashboard 默认大小
</commit_message>
<xml_diff>
--- a/src/main/resources/script/front/micro-service-init-data.xlsx
+++ b/src/main/resources/script/front/micro-service-init-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14540" tabRatio="800" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12660" tabRatio="800" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="IAM_PERMISSION" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="884" uniqueCount="376">
   <si>
     <t>IAM_PERMISSION</t>
   </si>
@@ -1052,7 +1052,7 @@
     <t>IS_ENABLED</t>
   </si>
   <si>
-    <t>@POSITION</t>
+    <t>POSITION</t>
   </si>
   <si>
     <t>ProjectInfo</t>
@@ -1083,9 +1083,6 @@
   </si>
   <si>
     <t>domain</t>
-  </si>
-  <si>
-    <t>{"width": 4, "positionX": 0, "positionY": 0, "height": 3}</t>
   </si>
   <si>
     <t>Announcement</t>
@@ -1197,8 +1194,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1235,9 +1232,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1251,23 +1262,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1275,13 +1272,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1295,62 +1285,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1379,6 +1316,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="DejaVu Sans"/>
       <charset val="134"/>
@@ -1393,7 +1390,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1405,13 +1414,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1423,19 +1438,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1447,31 +1468,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1489,7 +1486,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1501,79 +1564,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1620,6 +1617,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1650,6 +1656,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1675,172 +1696,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2173,7 +2170,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="D7:O32"/>
   <sheetViews>
@@ -2181,18 +2178,18 @@
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="6" max="6" width="38.8897058823529" customWidth="1"/>
-    <col min="7" max="7" width="37.2205882352941" customWidth="1"/>
+    <col min="6" max="6" width="38.8857142857143" customWidth="1"/>
+    <col min="7" max="7" width="37.2190476190476" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="14.2205882352941" customWidth="1"/>
+    <col min="10" max="10" width="14.2190476190476" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
-    <col min="12" max="12" width="19.2205882352941" customWidth="1"/>
-    <col min="13" max="13" width="18.7794117647059" customWidth="1"/>
-    <col min="14" max="14" width="19.3308823529412" customWidth="1"/>
+    <col min="12" max="12" width="19.2190476190476" customWidth="1"/>
+    <col min="13" max="13" width="18.7809523809524" customWidth="1"/>
+    <col min="14" max="14" width="19.3333333333333" customWidth="1"/>
     <col min="15" max="15" width="19" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2984,24 +2981,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="D7:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L2" workbookViewId="0">
+    <sheetView topLeftCell="L2" workbookViewId="0">
       <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="4" max="4" width="15.2205882352941" customWidth="1"/>
-    <col min="6" max="6" width="46.7794117647059" customWidth="1"/>
-    <col min="7" max="7" width="16.7794117647059" customWidth="1"/>
+    <col min="4" max="4" width="15.2190476190476" customWidth="1"/>
+    <col min="6" max="6" width="46.7809523809524" customWidth="1"/>
+    <col min="7" max="7" width="16.7809523809524" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="63.8897058823529" customWidth="1"/>
-    <col min="10" max="10" width="18.5514705882353" customWidth="1"/>
-    <col min="11" max="11" width="29.2205882352941" customWidth="1"/>
-    <col min="12" max="12" width="19.2205882352941" customWidth="1"/>
+    <col min="9" max="9" width="63.8857142857143" customWidth="1"/>
+    <col min="10" max="10" width="18.552380952381" customWidth="1"/>
+    <col min="11" max="11" width="29.2190476190476" customWidth="1"/>
+    <col min="12" max="12" width="19.2190476190476" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" ht="12.75" customHeight="1" spans="4:17">
@@ -4057,7 +4054,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="D7:H131"/>
   <sheetViews>
@@ -4065,10 +4062,10 @@
       <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="4" max="4" width="23.7794117647059" customWidth="1"/>
-    <col min="6" max="6" width="36.6617647058824" customWidth="1"/>
+    <col min="4" max="4" width="23.7809523809524" customWidth="1"/>
+    <col min="6" max="6" width="36.6571428571429" customWidth="1"/>
     <col min="7" max="7" width="63" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5152,28 +5149,28 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="D7:U15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="3" width="11.6617647058824" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.2205882352941" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.2205882352941" style="2" customWidth="1"/>
-    <col min="6" max="6" width="23.4411764705882" style="2" customWidth="1"/>
-    <col min="7" max="8" width="23.8897058823529" style="2" customWidth="1"/>
+    <col min="1" max="3" width="11.6571428571429" style="2" customWidth="1"/>
+    <col min="4" max="4" width="18.2190476190476" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.2190476190476" style="2" customWidth="1"/>
+    <col min="6" max="6" width="23.4380952380952" style="2" customWidth="1"/>
+    <col min="7" max="8" width="23.8857142857143" style="2" customWidth="1"/>
     <col min="9" max="10" width="24" style="2" customWidth="1"/>
-    <col min="11" max="11" width="13.4411764705882" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.6617647058824" style="2" customWidth="1"/>
-    <col min="13" max="13" width="28.6617647058824" style="2" customWidth="1"/>
-    <col min="14" max="17" width="11.6617647058824" style="2" customWidth="1"/>
-    <col min="18" max="18" width="46.3308823529412" style="2" customWidth="1"/>
-    <col min="19" max="1025" width="11.6617647058824" style="2" customWidth="1"/>
+    <col min="11" max="11" width="13.4380952380952" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.6571428571429" style="2" customWidth="1"/>
+    <col min="13" max="13" width="28.6571428571429" style="2" customWidth="1"/>
+    <col min="14" max="17" width="11.6571428571429" style="2" customWidth="1"/>
+    <col min="18" max="18" width="46.3333333333333" style="2" customWidth="1"/>
+    <col min="19" max="1025" width="11.6571428571429" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="4:18">
@@ -5358,7 +5355,7 @@
         <v>1</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="S10"/>
       <c r="T10"/>
@@ -5366,22 +5363,22 @@
     </row>
     <row r="11" spans="5:21">
       <c r="E11" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>344</v>
-      </c>
       <c r="I11" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="J11" s="2" t="s">
         <v>343</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>344</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>333</v>
@@ -5390,10 +5387,10 @@
         <v>15</v>
       </c>
       <c r="M11" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="N11" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="N11" s="2" t="s">
-        <v>346</v>
       </c>
       <c r="O11" s="2">
         <v>3</v>
@@ -5405,7 +5402,7 @@
         <v>1</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="S11"/>
       <c r="T11"/>
@@ -5413,22 +5410,22 @@
     </row>
     <row r="12" spans="5:21">
       <c r="E12" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>348</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>349</v>
-      </c>
       <c r="I12" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>348</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>349</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>333</v>
@@ -5437,10 +5434,10 @@
         <v>15</v>
       </c>
       <c r="M12" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="N12" s="2" t="s">
         <v>350</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>351</v>
       </c>
       <c r="O12" s="2">
         <v>11</v>
@@ -5452,7 +5449,7 @@
         <v>1</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="S12"/>
       <c r="T12"/>
@@ -5460,22 +5457,22 @@
     </row>
     <row r="13" spans="5:21">
       <c r="E13" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>354</v>
-      </c>
       <c r="I13" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>353</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>354</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>333</v>
@@ -5484,7 +5481,7 @@
         <v>15</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="N13" s="2" t="s">
         <v>341</v>
@@ -5499,7 +5496,7 @@
         <v>1</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="S13"/>
       <c r="T13"/>
@@ -5507,22 +5504,22 @@
     </row>
     <row r="14" spans="5:21">
       <c r="E14" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>357</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>358</v>
-      </c>
       <c r="I14" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="J14" s="2" t="s">
         <v>357</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>358</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>333</v>
@@ -5531,10 +5528,10 @@
         <v>15</v>
       </c>
       <c r="M14" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="N14" s="2" t="s">
         <v>359</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>360</v>
       </c>
       <c r="O14" s="2">
         <v>9</v>
@@ -5546,7 +5543,7 @@
         <v>1</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="S14"/>
       <c r="T14"/>
@@ -5554,22 +5551,22 @@
     </row>
     <row r="15" spans="5:21">
       <c r="E15" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="I15" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>362</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>363</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>333</v>
@@ -5578,10 +5575,10 @@
         <v>15</v>
       </c>
       <c r="M15" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="N15" s="2" t="s">
         <v>364</v>
-      </c>
-      <c r="N15" s="2" t="s">
-        <v>365</v>
       </c>
       <c r="O15" s="2">
         <v>10</v>
@@ -5593,7 +5590,7 @@
         <v>1</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="S15"/>
       <c r="T15"/>
@@ -5607,7 +5604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="D7:G12"/>
   <sheetViews>
@@ -5615,68 +5612,68 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="3" width="11.5514705882353" style="2"/>
-    <col min="4" max="4" width="22.2205882352941" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.5514705882353" style="2"/>
-    <col min="6" max="6" width="24.4411764705882" style="2" customWidth="1"/>
-    <col min="7" max="7" width="28.4411764705882" style="2" customWidth="1"/>
-    <col min="8" max="1025" width="11.5514705882353" style="2"/>
+    <col min="1" max="3" width="11.552380952381" style="2"/>
+    <col min="4" max="4" width="22.2190476190476" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.552380952381" style="2"/>
+    <col min="6" max="6" width="24.4380952380952" style="2" customWidth="1"/>
+    <col min="7" max="7" width="28.4380952380952" style="2" customWidth="1"/>
+    <col min="8" max="1025" width="11.552380952381" style="2"/>
   </cols>
   <sheetData>
     <row r="7" spans="4:7">
       <c r="D7" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>368</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>369</v>
       </c>
     </row>
     <row r="8" spans="6:7">
       <c r="F8" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="9" spans="6:7">
       <c r="F9" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="10" spans="6:7">
       <c r="F10" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="11" spans="6:7">
       <c r="F11" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="12" spans="6:7">
       <c r="F12" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -5687,7 +5684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="D6:H26"/>
   <sheetViews>
@@ -5695,36 +5692,36 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88970588235294" defaultRowHeight="14" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="8.88571428571429" defaultRowHeight="14.25" outlineLevelCol="7"/>
   <cols>
-    <col min="4" max="4" width="34.2205882352941" customWidth="1"/>
-    <col min="5" max="5" width="18.8897058823529" customWidth="1"/>
-    <col min="6" max="6" width="15.3308823529412" customWidth="1"/>
-    <col min="7" max="7" width="38.5514705882353" customWidth="1"/>
-    <col min="8" max="8" width="16.8897058823529" customWidth="1"/>
+    <col min="4" max="4" width="34.2190476190476" customWidth="1"/>
+    <col min="5" max="5" width="18.8857142857143" customWidth="1"/>
+    <col min="6" max="6" width="15.3333333333333" customWidth="1"/>
+    <col min="7" max="7" width="38.552380952381" customWidth="1"/>
+    <col min="8" max="8" width="16.8857142857143" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" ht="14.75"/>
+    <row r="6" ht="15"/>
     <row r="7" ht="19.05" customHeight="1" spans="4:8">
       <c r="D7" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>371</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>372</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>212</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="6:8">
       <c r="F8" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G8" t="s">
         <v>141</v>
@@ -5735,7 +5732,7 @@
     </row>
     <row r="9" spans="6:8">
       <c r="F9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G9" t="s">
         <v>145</v>
@@ -5746,7 +5743,7 @@
     </row>
     <row r="10" spans="6:8">
       <c r="F10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G10" t="s">
         <v>149</v>
@@ -5757,7 +5754,7 @@
     </row>
     <row r="11" spans="6:8">
       <c r="F11" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G11" t="s">
         <v>153</v>
@@ -5768,7 +5765,7 @@
     </row>
     <row r="12" spans="6:8">
       <c r="F12" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G12" t="s">
         <v>155</v>
@@ -5779,7 +5776,7 @@
     </row>
     <row r="13" spans="6:8">
       <c r="F13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G13" t="s">
         <v>159</v>
@@ -5790,7 +5787,7 @@
     </row>
     <row r="14" spans="6:8">
       <c r="F14" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G14" t="s">
         <v>162</v>
@@ -5801,7 +5798,7 @@
     </row>
     <row r="15" spans="6:8">
       <c r="F15" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G15" t="s">
         <v>166</v>
@@ -5812,7 +5809,7 @@
     </row>
     <row r="16" spans="6:8">
       <c r="F16" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G16" t="s">
         <v>170</v>
@@ -5823,7 +5820,7 @@
     </row>
     <row r="17" spans="6:8">
       <c r="F17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G17" t="s">
         <v>174</v>
@@ -5834,40 +5831,40 @@
     </row>
     <row r="18" spans="6:8">
       <c r="F18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G18" t="s">
         <v>178</v>
       </c>
       <c r="H18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="19" spans="6:8">
       <c r="F19" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G19" t="s">
         <v>182</v>
       </c>
       <c r="H19" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="6:8">
       <c r="F20" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G20" t="s">
         <v>184</v>
       </c>
       <c r="H20" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="21" spans="6:8">
       <c r="F21" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G21" t="s">
         <v>178</v>
@@ -5878,7 +5875,7 @@
     </row>
     <row r="22" spans="6:8">
       <c r="F22" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G22" t="s">
         <v>182</v>
@@ -5889,7 +5886,7 @@
     </row>
     <row r="23" spans="6:8">
       <c r="F23" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G23" t="s">
         <v>184</v>

</xml_diff>